<commit_message>
update q17 code and metadata
</commit_message>
<xml_diff>
--- a/data/derived/public/Q17_coding.xlsx
+++ b/data/derived/public/Q17_coding.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Samsung_T5/Grants/2021-NSF-HEGS-R&amp;R/Annals of AAG - Replicability Survey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\hegsrr\OR-Replicability-in-Geography-Survey\data\derived\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD4351-6AF9-FE44-A6ED-1FC0EABB9EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="4040" windowWidth="27640" windowHeight="16940" xr2:uid="{57A4F024-5EBE-B743-AFE9-1371A635E548}"/>
+    <workbookView xWindow="2880" yWindow="4040" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="438">
   <si>
     <t>ResponseId</t>
   </si>
@@ -1339,16 +1338,40 @@
     <t>love this answer from a qualitative human geographer!</t>
   </si>
   <si>
-    <t>Wasn't part of the goal of that study.</t>
-  </si>
-  <si>
     <t>It depends, frankly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Q22_code</t>
+  </si>
+  <si>
+    <t>2, 1</t>
+  </si>
+  <si>
+    <t>1, 4</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>4, 6</t>
+  </si>
+  <si>
+    <t>5, 4</t>
+  </si>
+  <si>
+    <t>2, 6</t>
+  </si>
+  <si>
+    <t>3, 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1712,14 +1735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD60B12-CB6A-C34D-B549-908DD5915872}">
-  <dimension ref="A1:AD100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q95" sqref="Q95"/>
+    <sheetView tabSelected="1" topLeftCell="Y16" workbookViewId="0">
+      <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
@@ -1728,11 +1751,11 @@
     <col min="5" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="27" width="10.83203125" style="1"/>
-    <col min="28" max="28" width="60.1640625" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="1"/>
+    <col min="28" max="29" width="60.1640625" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1818,13 +1841,16 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1903,14 +1929,14 @@
       <c r="AB2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -1989,14 +2015,17 @@
       <c r="AB3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -2079,13 +2108,16 @@
         <v>63</v>
       </c>
       <c r="AC4" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>65</v>
       </c>
@@ -2164,14 +2196,17 @@
       <c r="AB5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -2250,14 +2285,17 @@
       <c r="AB6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AC6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -2336,14 +2374,17 @@
       <c r="AB7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AC7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -2422,14 +2463,14 @@
       <c r="AB8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AD8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AE8" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
@@ -2509,13 +2550,16 @@
         <v>89</v>
       </c>
       <c r="AC9" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="AD9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AE9" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
@@ -2595,13 +2639,16 @@
         <v>93</v>
       </c>
       <c r="AC10" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="AD10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AE10" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>95</v>
       </c>
@@ -2680,14 +2727,17 @@
       <c r="AB11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AE11" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -2766,14 +2816,17 @@
       <c r="AB12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC12" s="1" t="s">
+      <c r="AC12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD12" s="1" t="s">
+      <c r="AE12" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>101</v>
       </c>
@@ -2855,14 +2908,17 @@
       <c r="AB13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="AC13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="AE13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
@@ -2944,14 +3000,17 @@
       <c r="AB14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AC14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AE14" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>113</v>
       </c>
@@ -3031,13 +3090,16 @@
         <v>116</v>
       </c>
       <c r="AC15" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD15" s="1" t="s">
+      <c r="AE15" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>117</v>
       </c>
@@ -3122,14 +3184,17 @@
       <c r="AB16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AC16" s="1" t="s">
+      <c r="AC16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD16" s="1" t="s">
+      <c r="AE16" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>124</v>
       </c>
@@ -3210,14 +3275,17 @@
       <c r="AB17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AC17" s="1" t="s">
+      <c r="AC17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AE17" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -3296,14 +3364,14 @@
       <c r="AB18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AE18" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>133</v>
       </c>
@@ -3382,14 +3450,17 @@
       <c r="AB19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AC19" s="1" t="s">
+      <c r="AC19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD19" s="1" t="s">
+      <c r="AE19" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
@@ -3471,14 +3542,17 @@
       <c r="AB20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AC20" s="1" t="s">
+      <c r="AC20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>143</v>
       </c>
@@ -3557,14 +3631,17 @@
       <c r="AB21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AC21" s="1" t="s">
+      <c r="AC21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>148</v>
       </c>
@@ -3646,14 +3723,17 @@
       <c r="AB22" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AC22" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD22" s="1" t="s">
+      <c r="AE22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>153</v>
       </c>
@@ -3738,14 +3818,17 @@
       <c r="AB23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AC23" s="1" t="s">
+      <c r="AC23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD23" s="1" t="s">
+      <c r="AE23" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>158</v>
       </c>
@@ -3827,14 +3910,17 @@
       <c r="AB24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AC24" s="1" t="s">
+      <c r="AC24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD24" s="1" t="s">
+      <c r="AE24" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>163</v>
       </c>
@@ -3913,14 +3999,17 @@
       <c r="AB25" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AC25" s="1" t="s">
+      <c r="AC25" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD25" s="1" t="s">
+      <c r="AE25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="289" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="263.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>167</v>
       </c>
@@ -4003,14 +4092,17 @@
       <c r="AB26" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AC26" s="1" t="s">
+      <c r="AC26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD26" s="1" t="s">
+      <c r="AE26" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>173</v>
       </c>
@@ -4089,14 +4181,17 @@
       <c r="AB27" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AC27" s="1" t="s">
+      <c r="AC27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD27" s="1" t="s">
+      <c r="AE27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>177</v>
       </c>
@@ -4177,14 +4272,17 @@
       <c r="AB28" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AC28" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD28" s="1" t="s">
+      <c r="AE28" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>182</v>
       </c>
@@ -4263,14 +4361,14 @@
       <c r="AB29" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AC29" s="1" t="s">
+      <c r="AD29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD29" s="1" t="s">
+      <c r="AE29" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>186</v>
       </c>
@@ -4350,13 +4448,16 @@
         <v>189</v>
       </c>
       <c r="AC30" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AD30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD30" s="1" t="s">
+      <c r="AE30" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>190</v>
       </c>
@@ -4438,14 +4539,17 @@
       <c r="AB31" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AC31" s="1" t="s">
+      <c r="AC31" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD31" s="1" t="s">
+      <c r="AE31" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>196</v>
       </c>
@@ -4524,14 +4628,17 @@
       <c r="AB32" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AC32" s="1" t="s">
+      <c r="AC32" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD32" s="1" t="s">
+      <c r="AE32" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>200</v>
       </c>
@@ -4610,14 +4717,17 @@
       <c r="AB33" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AC33" s="1" t="s">
+      <c r="AC33" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD33" s="1" t="s">
+      <c r="AE33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>204</v>
       </c>
@@ -4696,14 +4806,14 @@
       <c r="AB34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC34" s="1" t="s">
+      <c r="AD34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD34" s="1" t="s">
+      <c r="AE34" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>206</v>
       </c>
@@ -4782,14 +4892,14 @@
       <c r="AB35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC35" s="1" t="s">
+      <c r="AD35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD35" s="1" t="s">
+      <c r="AE35" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>208</v>
       </c>
@@ -4871,14 +4981,14 @@
       <c r="AB36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC36" s="1" t="s">
+      <c r="AD36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD36" s="1" t="s">
+      <c r="AE36" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>212</v>
       </c>
@@ -4960,14 +5070,14 @@
       <c r="AB37" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC37" s="1" t="s">
+      <c r="AD37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD37" s="1" t="s">
+      <c r="AE37" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>216</v>
       </c>
@@ -5049,14 +5159,14 @@
       <c r="AB38" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC38" s="1" t="s">
+      <c r="AD38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD38" s="1" t="s">
+      <c r="AE38" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>220</v>
       </c>
@@ -5141,14 +5251,14 @@
       <c r="AB39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC39" s="1" t="s">
+      <c r="AD39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD39" s="1" t="s">
+      <c r="AE39" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>225</v>
       </c>
@@ -5227,14 +5337,14 @@
       <c r="AB40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC40" s="1" t="s">
+      <c r="AD40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD40" s="1" t="s">
+      <c r="AE40" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>228</v>
       </c>
@@ -5313,14 +5423,14 @@
       <c r="AB41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC41" s="1" t="s">
+      <c r="AD41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD41" s="1" t="s">
+      <c r="AE41" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>231</v>
       </c>
@@ -5399,14 +5509,14 @@
       <c r="AB42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC42" s="1" t="s">
+      <c r="AD42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD42" s="1" t="s">
+      <c r="AE42" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>234</v>
       </c>
@@ -5485,14 +5595,14 @@
       <c r="AB43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC43" s="1" t="s">
+      <c r="AD43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD43" s="1" t="s">
+      <c r="AE43" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>236</v>
       </c>
@@ -5571,14 +5681,14 @@
       <c r="AB44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC44" s="1" t="s">
+      <c r="AD44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD44" s="1" t="s">
+      <c r="AE44" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>239</v>
       </c>
@@ -5657,14 +5767,14 @@
       <c r="AB45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC45" s="1" t="s">
+      <c r="AD45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD45" s="1" t="s">
+      <c r="AE45" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>242</v>
       </c>
@@ -5743,14 +5853,14 @@
       <c r="AB46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC46" s="1" t="s">
+      <c r="AD46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD46" s="1" t="s">
+      <c r="AE46" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>244</v>
       </c>
@@ -5829,14 +5939,14 @@
       <c r="AB47" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC47" s="1" t="s">
+      <c r="AD47" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD47" s="1" t="s">
+      <c r="AE47" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>247</v>
       </c>
@@ -5915,14 +6025,14 @@
       <c r="AB48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC48" s="1" t="s">
+      <c r="AD48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD48" s="1" t="s">
+      <c r="AE48" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>249</v>
       </c>
@@ -6001,14 +6111,14 @@
       <c r="AB49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC49" s="1" t="s">
+      <c r="AD49" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD49" s="1" t="s">
+      <c r="AE49" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>250</v>
       </c>
@@ -6087,14 +6197,14 @@
       <c r="AB50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC50" s="1" t="s">
+      <c r="AD50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD50" s="1" t="s">
+      <c r="AE50" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>252</v>
       </c>
@@ -6173,14 +6283,14 @@
       <c r="AB51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC51" s="1" t="s">
+      <c r="AD51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD51" s="1" t="s">
+      <c r="AE51" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>255</v>
       </c>
@@ -6259,14 +6369,14 @@
       <c r="AB52" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC52" s="1" t="s">
+      <c r="AD52" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD52" s="1" t="s">
+      <c r="AE52" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>257</v>
       </c>
@@ -6345,14 +6455,14 @@
       <c r="AB53" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC53" s="1" t="s">
+      <c r="AD53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD53" s="1" t="s">
+      <c r="AE53" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>259</v>
       </c>
@@ -6431,14 +6541,14 @@
       <c r="AB54" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC54" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD54" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE54" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>261</v>
       </c>
@@ -6517,14 +6627,14 @@
       <c r="AB55" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC55" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD55" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE55" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>263</v>
       </c>
@@ -6603,14 +6713,14 @@
       <c r="AB56" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC56" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD56" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE56" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>264</v>
       </c>
@@ -6689,14 +6799,14 @@
       <c r="AB57" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC57" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD57" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE57" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>265</v>
       </c>
@@ -6775,14 +6885,14 @@
       <c r="AB58" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC58" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD58" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE58" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>267</v>
       </c>
@@ -6861,14 +6971,14 @@
       <c r="AB59" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC59" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD59" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE59" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>268</v>
       </c>
@@ -6947,14 +7057,14 @@
       <c r="AB60" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC60" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AD60" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AE60" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>270</v>
       </c>
@@ -7033,14 +7143,14 @@
       <c r="AB61" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC61" s="1" t="s">
+      <c r="AD61" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD61" s="1" t="s">
+      <c r="AE61" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>272</v>
       </c>
@@ -7119,14 +7229,14 @@
       <c r="AB62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC62" s="1" t="s">
+      <c r="AD62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD62" s="1" t="s">
+      <c r="AE62" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>274</v>
       </c>
@@ -7205,14 +7315,14 @@
       <c r="AB63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC63" s="1" t="s">
+      <c r="AD63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD63" s="1" t="s">
+      <c r="AE63" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>276</v>
       </c>
@@ -7297,14 +7407,14 @@
       <c r="AB64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC64" s="1" t="s">
+      <c r="AD64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD64" s="1" t="s">
+      <c r="AE64" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>281</v>
       </c>
@@ -7383,14 +7493,14 @@
       <c r="AB65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC65" s="1" t="s">
+      <c r="AD65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD65" s="1" t="s">
+      <c r="AE65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>284</v>
       </c>
@@ -7469,14 +7579,14 @@
       <c r="AB66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC66" s="1" t="s">
+      <c r="AD66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD66" s="1" t="s">
+      <c r="AE66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>287</v>
       </c>
@@ -7555,14 +7665,14 @@
       <c r="AB67" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC67" s="1" t="s">
+      <c r="AD67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD67" s="1" t="s">
+      <c r="AE67" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>290</v>
       </c>
@@ -7641,14 +7751,14 @@
       <c r="AB68" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC68" s="1" t="s">
+      <c r="AD68" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD68" s="1" t="s">
+      <c r="AE68" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>292</v>
       </c>
@@ -7730,14 +7840,14 @@
       <c r="AB69" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC69" s="1" t="s">
+      <c r="AD69" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD69" s="1" t="s">
+      <c r="AE69" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>297</v>
       </c>
@@ -7819,14 +7929,14 @@
       <c r="AB70" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC70" s="1" t="s">
+      <c r="AD70" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD70" s="1" t="s">
+      <c r="AE70" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>302</v>
       </c>
@@ -7908,14 +8018,14 @@
       <c r="AB71" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC71" s="1" t="s">
+      <c r="AD71" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD71" s="1" t="s">
+      <c r="AE71" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>306</v>
       </c>
@@ -7994,14 +8104,14 @@
       <c r="AB72" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC72" s="1" t="s">
+      <c r="AD72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD72" s="1" t="s">
+      <c r="AE72" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>310</v>
       </c>
@@ -8080,14 +8190,14 @@
       <c r="AB73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC73" s="1" t="s">
+      <c r="AD73" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD73" s="1" t="s">
+      <c r="AE73" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>314</v>
       </c>
@@ -8166,14 +8276,14 @@
       <c r="AB74" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC74" s="1" t="s">
+      <c r="AD74" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD74" s="1" t="s">
+      <c r="AE74" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -8252,14 +8362,14 @@
       <c r="AB75" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC75" s="1" t="s">
+      <c r="AD75" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD75" s="1" t="s">
+      <c r="AE75" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>321</v>
       </c>
@@ -8338,14 +8448,14 @@
       <c r="AB76" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC76" s="1" t="s">
+      <c r="AD76" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD76" s="1" t="s">
+      <c r="AE76" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>325</v>
       </c>
@@ -8424,14 +8534,14 @@
       <c r="AB77" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC77" s="1" t="s">
+      <c r="AD77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD77" s="1" t="s">
+      <c r="AE77" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>329</v>
       </c>
@@ -8510,14 +8620,14 @@
       <c r="AB78" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC78" s="1" t="s">
+      <c r="AD78" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD78" s="1" t="s">
+      <c r="AE78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>332</v>
       </c>
@@ -8596,14 +8706,14 @@
       <c r="AB79" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC79" s="1" t="s">
+      <c r="AD79" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD79" s="1" t="s">
+      <c r="AE79" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>333</v>
       </c>
@@ -8685,14 +8795,14 @@
       <c r="AB80" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC80" s="1" t="s">
+      <c r="AD80" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD80" s="1" t="s">
+      <c r="AE80" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>337</v>
       </c>
@@ -8774,14 +8884,17 @@
       <c r="AB81" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AC81" s="1" t="s">
+      <c r="AC81" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD81" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD81" s="1" t="s">
+      <c r="AE81" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>342</v>
       </c>
@@ -8864,14 +8977,17 @@
       <c r="AB82" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="AC82" s="1" t="s">
+      <c r="AC82" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD82" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD82" s="1" t="s">
+      <c r="AE82" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>348</v>
       </c>
@@ -8950,14 +9066,17 @@
       <c r="AB83" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AC83" s="1" t="s">
+      <c r="AC83" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD83" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD83" s="1" t="s">
+      <c r="AE83" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>350</v>
       </c>
@@ -9036,14 +9155,17 @@
       <c r="AB84" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AC84" s="1" t="s">
+      <c r="AC84" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD84" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD84" s="1" t="s">
+      <c r="AE84" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>353</v>
       </c>
@@ -9122,14 +9244,17 @@
       <c r="AB85" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="AC85" s="1" t="s">
+      <c r="AC85" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD85" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD85" s="1" t="s">
+      <c r="AE85" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>357</v>
       </c>
@@ -9211,14 +9336,17 @@
       <c r="AB86" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="AC86" s="1" t="s">
+      <c r="AC86" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD86" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD86" s="2" t="s">
+      <c r="AE86" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>363</v>
       </c>
@@ -9298,13 +9426,16 @@
         <v>366</v>
       </c>
       <c r="AC87" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="AD87" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD87" s="1" t="s">
+      <c r="AE87" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>368</v>
       </c>
@@ -9386,14 +9517,17 @@
       <c r="AB88" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="AC88" s="1" t="s">
+      <c r="AC88" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD88" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD88" s="1" t="s">
+      <c r="AE88" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>374</v>
       </c>
@@ -9472,14 +9606,17 @@
       <c r="AB89" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="AC89" s="1" t="s">
+      <c r="AC89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD89" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD89" s="1" t="s">
+      <c r="AE89" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>379</v>
       </c>
@@ -9558,14 +9695,17 @@
       <c r="AB90" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="AC90" s="1" t="s">
+      <c r="AC90" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD90" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD90" s="1" t="s">
+      <c r="AE90" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>384</v>
       </c>
@@ -9644,14 +9784,17 @@
       <c r="AB91" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="AC91" s="1" t="s">
+      <c r="AC91" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD91" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD91" s="1" t="s">
+      <c r="AE91" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>388</v>
       </c>
@@ -9730,14 +9873,17 @@
       <c r="AB92" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="AC92" s="1" t="s">
+      <c r="AC92" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD92" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD92" s="1" t="s">
+      <c r="AE92" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>393</v>
       </c>
@@ -9820,13 +9966,16 @@
         <v>397</v>
       </c>
       <c r="AC93" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="AD93" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD93" s="1" t="s">
+      <c r="AE93" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>399</v>
       </c>
@@ -9905,14 +10054,17 @@
       <c r="AB94" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="AC94" s="1" t="s">
+      <c r="AC94" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD94" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD94" s="1" t="s">
+      <c r="AE94" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>403</v>
       </c>
@@ -9993,14 +10145,17 @@
       <c r="AB95" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="AC95" s="1" t="s">
+      <c r="AC95" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD95" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD95" s="1" t="s">
+      <c r="AE95" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>407</v>
       </c>
@@ -10079,14 +10234,17 @@
       <c r="AB96" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="AC96" s="1" t="s">
+      <c r="AC96" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD96" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD96" s="1" t="s">
+      <c r="AE96" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>411</v>
       </c>
@@ -10168,14 +10326,17 @@
       <c r="AB97" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="AC97" s="1" t="s">
+      <c r="AC97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD97" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD97" s="1" t="s">
+      <c r="AE97" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>415</v>
       </c>
@@ -10257,14 +10418,17 @@
       <c r="AB98" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="AC98" s="1" t="s">
+      <c r="AC98" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD98" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD98" s="1" t="s">
+      <c r="AE98" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>420</v>
       </c>
@@ -10343,14 +10507,17 @@
       <c r="AB99" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="AC99" s="1" t="s">
+      <c r="AC99" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD99" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD99" s="1" t="s">
+      <c r="AE99" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>424</v>
       </c>
@@ -10430,13 +10597,13 @@
         <v>52</v>
       </c>
       <c r="AB100" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD100" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE100" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="AC100" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD100" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>